<commit_message>
added biter killing bounty
fixed science recipe missing names and animation oddity
</commit_message>
<xml_diff>
--- a/notes/biter coin values.xlsx
+++ b/notes/biter coin values.xlsx
@@ -27,12 +27,6 @@
     <t>m</t>
   </si>
   <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>health</t>
   </si>
   <si>
@@ -61,6 +55,12 @@
   </si>
   <si>
     <t>cube root, /2</t>
+  </si>
+  <si>
+    <t>big</t>
+  </si>
+  <si>
+    <t>behemoth</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,6 +412,7 @@
     <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -419,25 +420,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -452,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <f>SQRT(B2)/2</f>
+        <f t="shared" ref="D2:D8" si="0">SQRT(B2)/2</f>
         <v>1.9364916731037085</v>
       </c>
       <c r="E2" s="2">
@@ -468,7 +469,7 @@
         <v>1.0137003325955665</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H4" si="0">POWER(B2,(1/3)) /2</f>
+        <f t="shared" ref="H2:H4" si="1">POWER(B2,(1/3)) /2</f>
         <v>1.2331060371652351</v>
       </c>
     </row>
@@ -480,87 +481,87 @@
         <v>75</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C8" si="1">B3/15</f>
+        <f t="shared" ref="C3:C8" si="2">B3/15</f>
         <v>5</v>
       </c>
       <c r="D3" s="1">
-        <f>SQRT(B3)/2</f>
+        <f t="shared" si="0"/>
         <v>4.3301270189221936</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E8" si="2">FLOOR(SQRT(B3)/2,1)</f>
+        <f t="shared" ref="E3:E8" si="3">FLOOR(SQRT(B3)/2,1)</f>
         <v>4</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F8" si="3">POWER(B3,(1/3))</f>
+        <f t="shared" ref="F3:F8" si="4">POWER(B3,(1/3))</f>
         <v>4.2171633265087456</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G8" si="4">((100/F3)*B3 / 600)</f>
+        <f t="shared" ref="G3:G8" si="5">((100/F3)*B3 / 600)</f>
         <v>2.9640777537417193</v>
       </c>
       <c r="H3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1085816632543728</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>375</v>
       </c>
       <c r="C4">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>9.6824583655185421</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="4"/>
+        <v>7.2112478515370402</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="5"/>
+        <v>8.6670159293829361</v>
+      </c>
+      <c r="H4">
         <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="D4" s="1">
-        <f>SQRT(B4)/2</f>
-        <v>9.6824583655185421</v>
-      </c>
-      <c r="E4" s="2">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="3"/>
-        <v>7.2112478515370402</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="4"/>
-        <v>8.6670159293829361</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="0"/>
         <v>3.6056239257685201</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>3000</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="D5" s="1">
-        <f>SQRT(B5)/2</f>
+        <f t="shared" si="0"/>
         <v>27.386127875258307</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="F5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14.422495703074075</v>
       </c>
       <c r="G5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>34.668063717531759</v>
       </c>
       <c r="H5">
@@ -570,97 +571,97 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>6000</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>400</v>
       </c>
       <c r="D6" s="1">
-        <f>SQRT(B6)/2</f>
+        <f t="shared" si="0"/>
         <v>38.729833462074168</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="F6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18.171205928321388</v>
       </c>
       <c r="G6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>55.032120814910471</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H8" si="5">POWER(B6,(1/3)) /2</f>
+        <f t="shared" ref="H6:H8" si="6">POWER(B6,(1/3)) /2</f>
         <v>9.0856029641606941</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>12000</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>800</v>
       </c>
       <c r="D7" s="1">
-        <f>SQRT(B7)/2</f>
+        <f t="shared" si="0"/>
         <v>54.772255750516614</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="F7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22.894284851066633</v>
       </c>
       <c r="G7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>87.358046473629898</v>
       </c>
       <c r="H7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11.447142425533317</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>30000</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="D8" s="1">
-        <f>SQRT(B8)/2</f>
+        <f t="shared" si="0"/>
         <v>86.602540378443862</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>86</v>
       </c>
       <c r="F8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>31.072325059538588</v>
       </c>
       <c r="G8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>160.91489743427164</v>
       </c>
       <c r="H8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15.536162529769294</v>
       </c>
     </row>

</xml_diff>